<commit_message>
Bump ISS version to 3.0.4
</commit_message>
<xml_diff>
--- a/tests/SENIOR-Team_Free-PRELIMS-OCC-.xlsx
+++ b/tests/SENIOR-Team_Free-PRELIMS-OCC-.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leahy\RustroverProjects\check_cards\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEA27DA-F359-47EE-A935-F6339C8321DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5DD76B-DE0C-4FCA-A8E1-79D7658F4B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8987486B-5DC1-406A-92BD-FEEC5C92F2E7}"/>
   </bookViews>
@@ -243,13 +243,13 @@
     <t xml:space="preserve"> C4 C4 C4 RD2 S1</t>
   </si>
   <si>
-    <t>ISS Coach Card Version: 3.0.3</t>
-  </si>
-  <si>
     <t>C-Thr^2F-Forw-ow/2ln</t>
   </si>
   <si>
     <t xml:space="preserve"> A3a A6 A1c A6 F4f*0.3 F4e*0.5 F4f*0.5 F4f A1d</t>
+  </si>
+  <si>
+    <t>ISS Coach Card Version: 3.0.4</t>
   </si>
 </sst>
 </file>
@@ -434,16 +434,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -457,6 +447,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D3D526-A40C-4C69-8373-29C6A2FBDE73}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,96 +809,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -913,16 +913,16 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" ht="29.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -1016,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>43</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1620,6 +1620,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="A1:H1"/>
@@ -1627,13 +1634,6 @@
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:H3"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="6.9444444444444441E-3" right="6.9444444444444441E-3" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add a warning for A4b
</commit_message>
<xml_diff>
--- a/tests/SENIOR-Team_Free-PRELIMS-OCC-.xlsx
+++ b/tests/SENIOR-Team_Free-PRELIMS-OCC-.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leahy\RustroverProjects\check_cards\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5DD76B-DE0C-4FCA-A8E1-79D7658F4B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2F8E14-361B-4F1C-A71E-92AD1EAFE296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8987486B-5DC1-406A-92BD-FEEC5C92F2E7}"/>
   </bookViews>
@@ -192,9 +192,6 @@
     <t>2:30-2:45</t>
   </si>
   <si>
-    <t xml:space="preserve"> CB+ A4b 1RB A6 CB+ CB+ A1c 2RB</t>
-  </si>
-  <si>
     <t>940A</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>ISS Coach Card Version: 3.0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CB+ A5 1RB A6 CB+ CB+ A1c 2RB</t>
   </si>
 </sst>
 </file>
@@ -434,6 +434,16 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -447,16 +457,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,7 +794,7 @@
   <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,96 +809,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -913,16 +913,16 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="29.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -1016,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>39</v>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>43</v>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>47</v>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="11" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>39</v>
@@ -1213,12 +1213,12 @@
         <v>3.35</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>21</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>38</v>
@@ -1242,19 +1242,19 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="8">
         <v>2.5499999999999998</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>21</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>38</v>
@@ -1278,21 +1278,21 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="G28" s="8">
         <v>3.25</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1620,6 +1620,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:H3"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
@@ -1627,13 +1634,6 @@
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:H3"/>
   </mergeCells>
   <pageMargins left="6.9444444444444441E-3" right="6.9444444444444441E-3" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bump minimum ISS version to 3.0.5
</commit_message>
<xml_diff>
--- a/tests/SENIOR-Team_Free-PRELIMS-OCC-.xlsx
+++ b/tests/SENIOR-Team_Free-PRELIMS-OCC-.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leahy\RustroverProjects\check_cards\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2F8E14-361B-4F1C-A71E-92AD1EAFE296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F622788-5378-4F4A-A02F-48369857F54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8987486B-5DC1-406A-92BD-FEEC5C92F2E7}"/>
   </bookViews>
@@ -246,10 +246,10 @@
     <t xml:space="preserve"> A3a A6 A1c A6 F4f*0.3 F4e*0.5 F4f*0.5 F4f A1d</t>
   </si>
   <si>
-    <t>ISS Coach Card Version: 3.0.4</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CB+ A5 1RB A6 CB+ CB+ A1c 2RB</t>
+  </si>
+  <si>
+    <t>ISS Coach Card Version: 3.0.5</t>
   </si>
 </sst>
 </file>
@@ -434,16 +434,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -457,6 +447,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D3D526-A40C-4C69-8373-29C6A2FBDE73}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,96 +809,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -913,16 +913,16 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" ht="29.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>39</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1620,6 +1620,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="A1:H1"/>
@@ -1627,13 +1634,6 @@
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:H3"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="6.9444444444444441E-3" right="6.9444444444444441E-3" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>